<commit_message>
se redacta nuavemente la sección de propuesta de clusterización por FRE
</commit_message>
<xml_diff>
--- a/references/clusterRead.xlsx
+++ b/references/clusterRead.xlsx
@@ -1,21 +1,32 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" mc:Ignorable="x15 xr xr6 xr10">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="24430"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="24527"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Daniel\OneDrive\Documents\Trabajos\UAS-FNE-2\61_Regionalizacion\FRE_AnalisisEstadistico\references\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{5837469F-3D3D-4993-A4CB-DCF377BCF766}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8974ED89-6F37-4BCC-81AD-D131B3AB1D23}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11310"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11310" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="clusterRead" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="0"/>
+  <calcPr calcId="191029"/>
+  <extLst>
+    <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
+      <xcalcf:calcFeatures>
+        <xcalcf:feature name="microsoft.com:RD"/>
+        <xcalcf:feature name="microsoft.com:Single"/>
+        <xcalcf:feature name="microsoft.com:FV"/>
+        <xcalcf:feature name="microsoft.com:CNMTM"/>
+        <xcalcf:feature name="microsoft.com:LET_WF"/>
+      </xcalcf:calcFeatures>
+    </ext>
+  </extLst>
 </workbook>
 </file>
 
@@ -58,10 +69,9 @@
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
-  <numFmts count="2">
-    <numFmt numFmtId="169" formatCode="0.000"/>
-    <numFmt numFmtId="170" formatCode="0.0"/>
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
+  <numFmts count="1">
+    <numFmt numFmtId="164" formatCode="0.000"/>
   </numFmts>
   <fonts count="18" x14ac:knownFonts="1">
     <font>
@@ -540,15 +550,12 @@
     <xf numFmtId="0" fontId="1" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="1" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="8">
+  <cellXfs count="12">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="170" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="169" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="16" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
@@ -561,6 +568,21 @@
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="16" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="1" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="2" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="2" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
   </cellXfs>
@@ -917,11 +939,11 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:I7"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
+  <dimension ref="A1:I10"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="I7" sqref="A1:I7"/>
+      <selection activeCell="G3" sqref="G3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -937,46 +959,46 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A1" s="6" t="s">
+      <c r="A1" s="5" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="7" t="s">
+      <c r="B1" s="6" t="s">
         <v>9</v>
       </c>
-      <c r="C1" s="7"/>
-      <c r="D1" s="7"/>
-      <c r="E1" s="7"/>
-      <c r="F1" s="7" t="s">
+      <c r="C1" s="6"/>
+      <c r="D1" s="6"/>
+      <c r="E1" s="6"/>
+      <c r="F1" s="6" t="s">
         <v>10</v>
       </c>
-      <c r="G1" s="7"/>
-      <c r="H1" s="7"/>
-      <c r="I1" s="7"/>
+      <c r="G1" s="6"/>
+      <c r="H1" s="6"/>
+      <c r="I1" s="6"/>
     </row>
     <row r="2" spans="1:9" ht="34.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A2" s="6"/>
-      <c r="B2" s="4" t="s">
+      <c r="A2" s="5"/>
+      <c r="B2" s="3" t="s">
         <v>7</v>
       </c>
-      <c r="C2" s="4" t="s">
+      <c r="C2" s="3" t="s">
         <v>8</v>
       </c>
-      <c r="D2" s="4" t="s">
+      <c r="D2" s="3" t="s">
         <v>5</v>
       </c>
-      <c r="E2" s="4" t="s">
+      <c r="E2" s="3" t="s">
         <v>6</v>
       </c>
-      <c r="F2" s="4" t="s">
+      <c r="F2" s="3" t="s">
         <v>1</v>
       </c>
-      <c r="G2" s="4" t="s">
+      <c r="G2" s="3" t="s">
         <v>2</v>
       </c>
-      <c r="H2" s="4" t="s">
+      <c r="H2" s="3" t="s">
         <v>3</v>
       </c>
-      <c r="I2" s="4" t="s">
+      <c r="I2" s="3" t="s">
         <v>4</v>
       </c>
     </row>
@@ -984,57 +1006,57 @@
       <c r="A3" s="1">
         <v>1</v>
       </c>
-      <c r="B3" s="2">
-        <v>236.90909090909</v>
-      </c>
-      <c r="C3" s="2">
-        <v>29.7459429186036</v>
-      </c>
-      <c r="D3" s="5">
-        <v>23.363636363636299</v>
-      </c>
-      <c r="E3" s="3">
-        <v>0.64171122994652396</v>
-      </c>
-      <c r="F3" s="3">
-        <v>0.80063189407978697</v>
-      </c>
-      <c r="G3" s="3">
-        <v>0.96590909090909005</v>
-      </c>
-      <c r="H3" s="3">
-        <v>0.60606060606060597</v>
-      </c>
-      <c r="I3" s="3">
-        <v>11.5475091763085</v>
+      <c r="B3" s="4">
+        <v>475.5</v>
+      </c>
+      <c r="C3" s="4">
+        <v>71.447478785000001</v>
+      </c>
+      <c r="D3" s="4">
+        <v>91</v>
+      </c>
+      <c r="E3" s="9">
+        <v>0.76470588235294101</v>
+      </c>
+      <c r="F3" s="2">
+        <v>0.88743369638835001</v>
+      </c>
+      <c r="G3" s="9">
+        <v>0.75</v>
+      </c>
+      <c r="H3" s="9">
+        <v>0.41666666666666602</v>
+      </c>
+      <c r="I3" s="2">
+        <v>7.6541100000000002</v>
       </c>
     </row>
     <row r="4" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A4" s="1">
         <v>2</v>
       </c>
-      <c r="B4" s="2">
+      <c r="B4" s="4">
         <v>2714</v>
       </c>
-      <c r="C4" s="2">
+      <c r="C4" s="4">
         <v>978.38835269000003</v>
       </c>
-      <c r="D4" s="5">
+      <c r="D4" s="4">
         <v>1054</v>
       </c>
-      <c r="E4" s="3">
+      <c r="E4" s="9">
         <v>1</v>
       </c>
-      <c r="F4" s="3">
+      <c r="F4" s="2">
         <v>0.96164976306739802</v>
       </c>
-      <c r="G4" s="3">
+      <c r="G4" s="9">
         <v>1</v>
       </c>
-      <c r="H4" s="3">
+      <c r="H4" s="9">
         <v>1</v>
       </c>
-      <c r="I4" s="3">
+      <c r="I4" s="2">
         <v>8.1818181818181804E-2</v>
       </c>
     </row>
@@ -1042,87 +1064,174 @@
       <c r="A5" s="1">
         <v>3</v>
       </c>
-      <c r="B5" s="2">
-        <v>1237.25</v>
-      </c>
-      <c r="C5" s="2">
-        <v>97.485597526567503</v>
-      </c>
-      <c r="D5" s="5">
-        <v>181.625</v>
-      </c>
-      <c r="E5" s="3">
-        <v>0.91176470588235203</v>
-      </c>
-      <c r="F5" s="3">
-        <v>0.76420510791351803</v>
-      </c>
-      <c r="G5" s="3">
+      <c r="B5" s="4">
+        <v>821.93333333333305</v>
+      </c>
+      <c r="C5" s="4">
+        <v>80.272733311636003</v>
+      </c>
+      <c r="D5" s="4">
+        <v>149.933333333333</v>
+      </c>
+      <c r="E5" s="9">
+        <v>0.91764705882352904</v>
+      </c>
+      <c r="F5" s="2">
+        <v>0.96146745545502599</v>
+      </c>
+      <c r="G5" s="9">
         <v>1</v>
       </c>
-      <c r="H5" s="3">
-        <v>0.56249861111111099</v>
-      </c>
-      <c r="I5" s="3">
-        <v>25.418123749999999</v>
+      <c r="H5" s="9">
+        <v>0.54814740740740697</v>
+      </c>
+      <c r="I5" s="2">
+        <v>0.91869512254752705</v>
       </c>
     </row>
     <row r="6" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A6" s="1">
         <v>4</v>
       </c>
-      <c r="B6" s="2">
-        <v>756.3</v>
-      </c>
-      <c r="C6" s="2">
-        <v>74.8841112211</v>
-      </c>
-      <c r="D6" s="5">
-        <v>160.5</v>
-      </c>
-      <c r="E6" s="3">
-        <v>0.95294117647058796</v>
-      </c>
-      <c r="F6" s="3">
-        <v>0.88483001093829705</v>
-      </c>
-      <c r="G6" s="3">
-        <v>0.96250000000000002</v>
-      </c>
-      <c r="H6" s="3">
-        <v>0.39444444444444399</v>
-      </c>
-      <c r="I6" s="3">
-        <v>0.777965632539239</v>
+      <c r="B6" s="4">
+        <v>1252</v>
+      </c>
+      <c r="C6" s="4">
+        <v>15.5245885625</v>
+      </c>
+      <c r="D6" s="4">
+        <v>90.5</v>
+      </c>
+      <c r="E6" s="9">
+        <v>0.94117647058823495</v>
+      </c>
+      <c r="F6" s="2">
+        <v>0.80235460422413496</v>
+      </c>
+      <c r="G6" s="9">
+        <v>1</v>
+      </c>
+      <c r="H6" s="9">
+        <v>0.47222222222222199</v>
+      </c>
+      <c r="I6" s="2">
+        <v>100</v>
       </c>
     </row>
     <row r="7" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A7" s="1">
         <v>5</v>
       </c>
-      <c r="B7" s="2">
-        <v>2006</v>
-      </c>
-      <c r="C7" s="2">
-        <v>381.45676398400002</v>
-      </c>
-      <c r="D7" s="5">
-        <v>570</v>
-      </c>
-      <c r="E7" s="3">
+      <c r="B7" s="4">
+        <v>615.33333333333303</v>
+      </c>
+      <c r="C7" s="4">
+        <v>57.380750808333296</v>
+      </c>
+      <c r="D7" s="4">
+        <v>101.333333333333</v>
+      </c>
+      <c r="E7" s="9">
+        <v>0.88235294117647001</v>
+      </c>
+      <c r="F7" s="2">
+        <v>0.209039759485211</v>
+      </c>
+      <c r="G7" s="9">
+        <v>0.95833333333333304</v>
+      </c>
+      <c r="H7" s="9">
+        <v>0.74074074074074003</v>
+      </c>
+      <c r="I7" s="2">
+        <v>0.48735538461538402</v>
+      </c>
+    </row>
+    <row r="8" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A8" s="7">
+        <v>6</v>
+      </c>
+      <c r="B8" s="8">
+        <v>102</v>
+      </c>
+      <c r="C8" s="8">
+        <v>38.902520000000003</v>
+      </c>
+      <c r="D8" s="7">
         <v>1</v>
       </c>
-      <c r="F7" s="3">
-        <v>0.99950865290522795</v>
-      </c>
-      <c r="G7" s="3">
+      <c r="E8" s="10">
+        <v>0.58823529411764697</v>
+      </c>
+      <c r="F8" s="11">
+        <v>0</v>
+      </c>
+      <c r="G8" s="10">
+        <v>0.875</v>
+      </c>
+      <c r="H8" s="10">
+        <v>0.88888888888888795</v>
+      </c>
+      <c r="I8" s="11">
+        <v>90</v>
+      </c>
+    </row>
+    <row r="9" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A9" s="7">
+        <v>7</v>
+      </c>
+      <c r="B9" s="8">
+        <v>201.4</v>
+      </c>
+      <c r="C9" s="8">
+        <v>19.011901713127997</v>
+      </c>
+      <c r="D9" s="7">
+        <v>12.4</v>
+      </c>
+      <c r="E9" s="10">
+        <v>0.494117647058823</v>
+      </c>
+      <c r="F9" s="11">
+        <v>0.91935327750763396</v>
+      </c>
+      <c r="G9" s="10">
         <v>1</v>
       </c>
-      <c r="H7" s="3">
+      <c r="H9" s="10">
+        <v>0.4</v>
+      </c>
+      <c r="I9" s="11">
+        <v>3.4593068545454502</v>
+      </c>
+    </row>
+    <row r="10" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A10" s="7">
+        <v>8</v>
+      </c>
+      <c r="B10" s="8">
+        <v>1667</v>
+      </c>
+      <c r="C10" s="8">
+        <v>276.62430657599998</v>
+      </c>
+      <c r="D10" s="7">
+        <v>453</v>
+      </c>
+      <c r="E10" s="10">
+        <v>1</v>
+      </c>
+      <c r="F10" s="11">
+        <v>0.87146318071491902</v>
+      </c>
+      <c r="G10" s="10">
+        <v>1</v>
+      </c>
+      <c r="H10" s="10">
         <v>0</v>
       </c>
-      <c r="I7" s="3">
-        <v>5.348E-2</v>
+      <c r="I10" s="11">
+        <v>0.17674000000000001</v>
       </c>
     </row>
   </sheetData>
@@ -1131,7 +1240,7 @@
     <mergeCell ref="B1:E1"/>
     <mergeCell ref="F1:I1"/>
   </mergeCells>
-  <conditionalFormatting sqref="I3:I7">
+  <conditionalFormatting sqref="I3:I10">
     <cfRule type="colorScale" priority="8">
       <colorScale>
         <cfvo type="min"/>
@@ -1143,7 +1252,7 @@
       </colorScale>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="F3:F7">
+  <conditionalFormatting sqref="F3:F10">
     <cfRule type="colorScale" priority="7">
       <colorScale>
         <cfvo type="min"/>
@@ -1155,7 +1264,7 @@
       </colorScale>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="G3:G7">
+  <conditionalFormatting sqref="G3:G10">
     <cfRule type="colorScale" priority="6">
       <colorScale>
         <cfvo type="min"/>
@@ -1167,7 +1276,7 @@
       </colorScale>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="H3:H7">
+  <conditionalFormatting sqref="H3:H10">
     <cfRule type="colorScale" priority="5">
       <colorScale>
         <cfvo type="min"/>
@@ -1179,7 +1288,7 @@
       </colorScale>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="E3:E7">
+  <conditionalFormatting sqref="E3:E10">
     <cfRule type="colorScale" priority="4">
       <colorScale>
         <cfvo type="min"/>
@@ -1191,7 +1300,7 @@
       </colorScale>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="D3:D7">
+  <conditionalFormatting sqref="D3:D10">
     <cfRule type="colorScale" priority="3">
       <colorScale>
         <cfvo type="min"/>
@@ -1203,7 +1312,7 @@
       </colorScale>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="C3:C7">
+  <conditionalFormatting sqref="C3:C10">
     <cfRule type="colorScale" priority="2">
       <colorScale>
         <cfvo type="min"/>
@@ -1215,7 +1324,7 @@
       </colorScale>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="B3:B7">
+  <conditionalFormatting sqref="B3:B10">
     <cfRule type="colorScale" priority="1">
       <colorScale>
         <cfvo type="min"/>

</xml_diff>